<commit_message>
Migrated all tokens / snippets we had previously incl. datetime, etc.
</commit_message>
<xml_diff>
--- a/src/sxc-designer/source-editor/snippets.xlsx
+++ b/src/sxc-designer/source-editor/snippets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="464">
   <si>
     <t>set</t>
   </si>
@@ -962,9 +962,6 @@
     <t>Portal</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Profile</t>
   </si>
   <si>
@@ -1149,6 +1146,276 @@
   </si>
   <si>
     <t>Folder</t>
+  </si>
+  <si>
+    <t>[Tab:Description]</t>
+  </si>
+  <si>
+    <t>Page Description Text for Search Engine</t>
+  </si>
+  <si>
+    <t>[Tab:EndDate]</t>
+  </si>
+  <si>
+    <t>Page Display Until Date</t>
+  </si>
+  <si>
+    <t>[Tab:FullUrl]</t>
+  </si>
+  <si>
+    <t>Page Full URL</t>
+  </si>
+  <si>
+    <t>[Tab:IconFile]</t>
+  </si>
+  <si>
+    <t>Page Relative Path to Icon File</t>
+  </si>
+  <si>
+    <t>[Tab:KeyWords]</t>
+  </si>
+  <si>
+    <t>Page Keywords for Search Engine</t>
+  </si>
+  <si>
+    <t>[Tab:PageHeadText]</t>
+  </si>
+  <si>
+    <t>Page Header Text</t>
+  </si>
+  <si>
+    <t>[Tab:StartDate]</t>
+  </si>
+  <si>
+    <t>Page Display from Date</t>
+  </si>
+  <si>
+    <t>[Tab:TabName]</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>[Tab:TabPath]</t>
+  </si>
+  <si>
+    <t>Page Relative Path</t>
+  </si>
+  <si>
+    <t>[Tab:Title]</t>
+  </si>
+  <si>
+    <t>Page Title (Window Title)</t>
+  </si>
+  <si>
+    <t>[Tab:URL]</t>
+  </si>
+  <si>
+    <t>Page URL</t>
+  </si>
+  <si>
+    <t>[Module:Description]</t>
+  </si>
+  <si>
+    <t>Module Definition Description</t>
+  </si>
+  <si>
+    <t>[Module:EndDate]</t>
+  </si>
+  <si>
+    <t>Module Display Until Date</t>
+  </si>
+  <si>
+    <t>[Module:Footer]</t>
+  </si>
+  <si>
+    <t>Module Footer Text</t>
+  </si>
+  <si>
+    <t>[Module:FriendlyName]</t>
+  </si>
+  <si>
+    <t>Module Definition Name</t>
+  </si>
+  <si>
+    <t>[Module:Header]</t>
+  </si>
+  <si>
+    <t>Module Header Text</t>
+  </si>
+  <si>
+    <t>[Module:HelpURL]</t>
+  </si>
+  <si>
+    <t>Module Help URL</t>
+  </si>
+  <si>
+    <t>[Module:IconFile]</t>
+  </si>
+  <si>
+    <t>Module Path to Icon File</t>
+  </si>
+  <si>
+    <t>[Module:ModuleTitle]</t>
+  </si>
+  <si>
+    <t>Module Title</t>
+  </si>
+  <si>
+    <t>[Module:PaneName]</t>
+  </si>
+  <si>
+    <t>Module Name of Pane (where the module resides)</t>
+  </si>
+  <si>
+    <t>[Module:StartDate]</t>
+  </si>
+  <si>
+    <t>Module Display from Date</t>
+  </si>
+  <si>
+    <t>[QueryString:${1:ParameterName}]</t>
+  </si>
+  <si>
+    <t>Value of Querystring Name</t>
+  </si>
+  <si>
+    <t>[User:DisplayName]</t>
+  </si>
+  <si>
+    <t>User’s Display Name</t>
+  </si>
+  <si>
+    <t>[User:Email]</t>
+  </si>
+  <si>
+    <t>User’s Email Address</t>
+  </si>
+  <si>
+    <t>[User:FirstName]</t>
+  </si>
+  <si>
+    <t>User’s First Name</t>
+  </si>
+  <si>
+    <t>[User:FullName]</t>
+  </si>
+  <si>
+    <t>(deprecated)</t>
+  </si>
+  <si>
+    <t>[User:LastName]</t>
+  </si>
+  <si>
+    <t>User’s Last Name</t>
+  </si>
+  <si>
+    <t>[User:Username]</t>
+  </si>
+  <si>
+    <t>User’s Login User Name</t>
+  </si>
+  <si>
+    <t>[Profile:${1:City}]</t>
+  </si>
+  <si>
+    <t>Use any default or custom Profile Property as listed in Profile Property Definition section of Manage User Accounts. Use non-localized Property Name only.</t>
+  </si>
+  <si>
+    <t>[User</t>
+  </si>
+  <si>
+    <t>[Environment</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>FriendlyName</t>
+  </si>
+  <si>
+    <t>IconFile</t>
+  </si>
+  <si>
+    <t>HelpUrl</t>
+  </si>
+  <si>
+    <t>QueryString</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Difference in Minutes between Portal Default Time and UTC</t>
+  </si>
+  <si>
+    <t>Portal URL</t>
+  </si>
+  <si>
+    <t>Portal Name</t>
+  </si>
+  <si>
+    <t>Portal Path to Logo File</t>
+  </si>
+  <si>
+    <t>Portal Path (relative) of Home Directory</t>
+  </si>
+  <si>
+    <t>Portal Copyright Text</t>
+  </si>
+  <si>
+    <t>Portal Admin Email</t>
+  </si>
+  <si>
+    <t>Portal Description</t>
+  </si>
+  <si>
+    <t>Currency String</t>
+  </si>
+  <si>
+    <t>for automatic hiding of the page</t>
+  </si>
+  <si>
+    <t>@User</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>[DateTime:Now]</t>
+  </si>
+  <si>
+    <t>Current Date and Time</t>
+  </si>
+  <si>
+    <t>[Ticks:Now]</t>
+  </si>
+  <si>
+    <t>CPU Tick Count for Current Second</t>
+  </si>
+  <si>
+    <t>Ticks-Now</t>
+  </si>
+  <si>
+    <t>Ticks-Today</t>
+  </si>
+  <si>
+    <t>[Ticks:Today]</t>
+  </si>
+  <si>
+    <t>CPU Tick Count since Midnight</t>
+  </si>
+  <si>
+    <t>Ticks-Per-Day</t>
+  </si>
+  <si>
+    <t>[Ticks:TicksPerDay]</t>
+  </si>
+  <si>
+    <t>CPU Ticks per Day (for calculations)</t>
   </si>
 </sst>
 </file>
@@ -1205,8 +1472,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F225" totalsRowShown="0">
-  <autoFilter ref="A1:F225"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F217" totalsRowShown="0">
+  <autoFilter ref="A1:F217"/>
   <tableColumns count="6">
     <tableColumn id="1" name="set"/>
     <tableColumn id="7" name="subset"/>
@@ -1482,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F183"/>
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C175" sqref="C175"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="B213" sqref="B213:B216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1773,7 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -1520,7 +1787,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1540,7 +1807,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1560,7 +1827,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -1580,7 +1847,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -1600,7 +1867,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1620,7 +1887,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1640,13 +1907,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B8" t="s">
         <v>307</v>
       </c>
       <c r="C8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1654,13 +1921,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B9" t="s">
         <v>307</v>
       </c>
       <c r="C9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E9" t="s">
         <v>31</v>
@@ -1668,33 +1935,33 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B10" t="s">
         <v>308</v>
       </c>
       <c r="C10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" t="s">
         <v>308</v>
       </c>
       <c r="C11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -1702,7 +1969,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B12" t="s">
         <v>309</v>
@@ -1716,7 +1983,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B13" t="s">
         <v>309</v>
@@ -1730,7 +1997,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B14" t="s">
         <v>309</v>
@@ -1744,7 +2011,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B15" t="s">
         <v>309</v>
@@ -1758,7 +2025,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" t="s">
         <v>309</v>
@@ -1772,7 +2039,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B17" t="s">
         <v>309</v>
@@ -1786,7 +2053,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B18" t="s">
         <v>309</v>
@@ -1800,7 +2067,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B19" t="s">
         <v>309</v>
@@ -1814,7 +2081,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B20" t="s">
         <v>309</v>
@@ -1828,7 +2095,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B21" t="s">
         <v>309</v>
@@ -1842,7 +2109,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B22" t="s">
         <v>309</v>
@@ -1856,7 +2123,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B23" t="s">
         <v>309</v>
@@ -1870,7 +2137,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B24" t="s">
         <v>309</v>
@@ -1884,7 +2151,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B25" t="s">
         <v>309</v>
@@ -1898,7 +2165,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B26" t="s">
         <v>309</v>
@@ -1912,7 +2179,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B27" t="s">
         <v>309</v>
@@ -1926,7 +2193,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B28" t="s">
         <v>309</v>
@@ -1940,7 +2207,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B29" t="s">
         <v>309</v>
@@ -1954,7 +2221,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B30" t="s">
         <v>309</v>
@@ -1968,7 +2235,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B31" t="s">
         <v>309</v>
@@ -1982,7 +2249,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B32" t="s">
         <v>309</v>
@@ -1996,7 +2263,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B33" t="s">
         <v>309</v>
@@ -2010,7 +2277,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B34" t="s">
         <v>309</v>
@@ -2024,7 +2291,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B35" t="s">
         <v>309</v>
@@ -2038,7 +2305,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B36" t="s">
         <v>309</v>
@@ -2052,7 +2319,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B37" t="s">
         <v>309</v>
@@ -2066,7 +2333,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B38" t="s">
         <v>309</v>
@@ -2080,7 +2347,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B39" t="s">
         <v>309</v>
@@ -2094,7 +2361,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B40" t="s">
         <v>309</v>
@@ -2108,7 +2375,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B41" t="s">
         <v>309</v>
@@ -2122,7 +2389,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B42" t="s">
         <v>309</v>
@@ -2136,7 +2403,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B43" t="s">
         <v>309</v>
@@ -2150,7 +2417,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B44" t="s">
         <v>309</v>
@@ -2164,7 +2431,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B45" t="s">
         <v>309</v>
@@ -2178,7 +2445,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B46" t="s">
         <v>309</v>
@@ -2192,7 +2459,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B47" t="s">
         <v>309</v>
@@ -2206,7 +2473,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B48" t="s">
         <v>310</v>
@@ -2218,9 +2485,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B49" t="s">
         <v>310</v>
@@ -2232,9 +2499,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B50" t="s">
         <v>310</v>
@@ -2246,9 +2513,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B51" t="s">
         <v>310</v>
@@ -2260,9 +2527,9 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B52" t="s">
         <v>310</v>
@@ -2274,9 +2541,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B53" t="s">
         <v>310</v>
@@ -2288,9 +2555,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B54" t="s">
         <v>310</v>
@@ -2302,9 +2569,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B55" t="s">
         <v>310</v>
@@ -2315,10 +2582,13 @@
       <c r="E55" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B56" t="s">
         <v>310</v>
@@ -2330,9 +2600,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B57" t="s">
         <v>310</v>
@@ -2344,9 +2614,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B58" t="s">
         <v>310</v>
@@ -2358,9 +2628,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s">
         <v>310</v>
@@ -2372,9 +2642,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B60" t="s">
         <v>310</v>
@@ -2386,9 +2656,9 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B61" t="s">
         <v>310</v>
@@ -2400,9 +2670,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s">
         <v>310</v>
@@ -2414,9 +2684,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B63" t="s">
         <v>310</v>
@@ -2428,9 +2698,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B64" t="s">
         <v>310</v>
@@ -2444,7 +2714,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B65" t="s">
         <v>310</v>
@@ -2458,7 +2728,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B66" t="s">
         <v>310</v>
@@ -2472,7 +2742,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B67" t="s">
         <v>310</v>
@@ -2486,7 +2756,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B68" t="s">
         <v>310</v>
@@ -2500,7 +2770,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B69" t="s">
         <v>310</v>
@@ -2514,7 +2784,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B70" t="s">
         <v>310</v>
@@ -2528,7 +2798,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B71" t="s">
         <v>310</v>
@@ -2542,7 +2812,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B72" t="s">
         <v>310</v>
@@ -2556,7 +2826,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B73" t="s">
         <v>310</v>
@@ -2570,7 +2840,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B74" t="s">
         <v>310</v>
@@ -2584,7 +2854,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B75" t="s">
         <v>310</v>
@@ -2598,7 +2868,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B76" t="s">
         <v>310</v>
@@ -2612,7 +2882,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B77" t="s">
         <v>310</v>
@@ -2626,7 +2896,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B78" t="s">
         <v>310</v>
@@ -2640,7 +2910,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B79" t="s">
         <v>310</v>
@@ -2654,7 +2924,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B80" t="s">
         <v>310</v>
@@ -2668,7 +2938,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B81" t="s">
         <v>310</v>
@@ -2682,7 +2952,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B82" t="s">
         <v>310</v>
@@ -2696,7 +2966,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B83" t="s">
         <v>310</v>
@@ -2710,7 +2980,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B84" t="s">
         <v>310</v>
@@ -2724,7 +2994,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B85" t="s">
         <v>310</v>
@@ -2738,7 +3008,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B86" t="s">
         <v>310</v>
@@ -2752,7 +3022,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B87" t="s">
         <v>310</v>
@@ -2766,7 +3036,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B88" t="s">
         <v>310</v>
@@ -2780,7 +3050,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B89" t="s">
         <v>310</v>
@@ -2794,7 +3064,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B90" t="s">
         <v>311</v>
@@ -2808,7 +3078,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B91" t="s">
         <v>311</v>
@@ -2822,7 +3092,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B92" t="s">
         <v>311</v>
@@ -2836,7 +3106,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B93" t="s">
         <v>311</v>
@@ -2850,7 +3120,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B94" t="s">
         <v>311</v>
@@ -2864,7 +3134,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B95" t="s">
         <v>311</v>
@@ -2878,7 +3148,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B96" t="s">
         <v>311</v>
@@ -2892,7 +3162,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B97" t="s">
         <v>311</v>
@@ -2904,12 +3174,12 @@
         <v>197</v>
       </c>
       <c r="F97" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B98" t="s">
         <v>311</v>
@@ -2921,12 +3191,12 @@
         <v>199</v>
       </c>
       <c r="F98" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B99" t="s">
         <v>311</v>
@@ -2940,7 +3210,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B100" t="s">
         <v>311</v>
@@ -2954,7 +3224,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B101" t="s">
         <v>311</v>
@@ -2968,7 +3238,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B102" t="s">
         <v>311</v>
@@ -2982,7 +3252,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B103" t="s">
         <v>311</v>
@@ -2996,7 +3266,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B104" t="s">
         <v>311</v>
@@ -3010,7 +3280,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B105" t="s">
         <v>311</v>
@@ -3024,7 +3294,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B106" t="s">
         <v>311</v>
@@ -3038,7 +3308,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B107" t="s">
         <v>311</v>
@@ -3052,7 +3322,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B108" t="s">
         <v>311</v>
@@ -3066,7 +3336,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B109" t="s">
         <v>311</v>
@@ -3080,7 +3350,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B110" t="s">
         <v>311</v>
@@ -3094,7 +3364,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B111" t="s">
         <v>311</v>
@@ -3108,7 +3378,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B112" t="s">
         <v>311</v>
@@ -3120,12 +3390,12 @@
         <v>226</v>
       </c>
       <c r="F112" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B113" t="s">
         <v>311</v>
@@ -3139,7 +3409,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B114" t="s">
         <v>311</v>
@@ -3151,12 +3421,12 @@
         <v>229</v>
       </c>
       <c r="F114" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B115" t="s">
         <v>311</v>
@@ -3170,7 +3440,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B116" t="s">
         <v>311</v>
@@ -3184,7 +3454,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B117" t="s">
         <v>311</v>
@@ -3198,7 +3468,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B118" t="s">
         <v>311</v>
@@ -3212,7 +3482,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B119" t="s">
         <v>311</v>
@@ -3226,7 +3496,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B120" t="s">
         <v>311</v>
@@ -3240,7 +3510,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B121" t="s">
         <v>311</v>
@@ -3254,7 +3524,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B122" t="s">
         <v>311</v>
@@ -3268,7 +3538,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B123" t="s">
         <v>311</v>
@@ -3282,7 +3552,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B124" t="s">
         <v>311</v>
@@ -3294,12 +3564,12 @@
         <v>249</v>
       </c>
       <c r="F124" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B125" t="s">
         <v>311</v>
@@ -3313,7 +3583,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B126" t="s">
         <v>311</v>
@@ -3327,7 +3597,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B127" t="s">
         <v>311</v>
@@ -3341,7 +3611,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B128" t="s">
         <v>311</v>
@@ -3355,7 +3625,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B129" t="s">
         <v>311</v>
@@ -3369,7 +3639,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B130" t="s">
         <v>311</v>
@@ -3383,7 +3653,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B131" t="s">
         <v>311</v>
@@ -3397,7 +3667,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B132" t="s">
         <v>311</v>
@@ -3411,7 +3681,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B133" t="s">
         <v>311</v>
@@ -3425,7 +3695,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B134" t="s">
         <v>311</v>
@@ -3439,7 +3709,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B135" t="s">
         <v>311</v>
@@ -3453,7 +3723,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B136" t="s">
         <v>311</v>
@@ -3467,7 +3737,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B137" t="s">
         <v>311</v>
@@ -3481,7 +3751,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B138" t="s">
         <v>311</v>
@@ -3495,7 +3765,7 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B139" t="s">
         <v>311</v>
@@ -3509,7 +3779,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B140" t="s">
         <v>311</v>
@@ -3523,10 +3793,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B141" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C141" t="s">
         <v>282</v>
@@ -3537,10 +3807,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B142" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C142" t="s">
         <v>209</v>
@@ -3551,10 +3821,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B143" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C143" t="s">
         <v>285</v>
@@ -3565,10 +3835,10 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B144" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C144" t="s">
         <v>287</v>
@@ -3579,10 +3849,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B145" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C145" t="s">
         <v>125</v>
@@ -3593,10 +3863,10 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B146" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C146" t="s">
         <v>290</v>
@@ -3607,10 +3877,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B147" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C147" t="s">
         <v>292</v>
@@ -3621,10 +3891,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B148" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C148" t="s">
         <v>294</v>
@@ -3635,10 +3905,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B149" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C149" t="s">
         <v>296</v>
@@ -3647,15 +3917,15 @@
         <v>297</v>
       </c>
       <c r="F149" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B150" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C150" t="s">
         <v>236</v>
@@ -3666,10 +3936,10 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B151" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C151" t="s">
         <v>299</v>
@@ -3678,15 +3948,15 @@
         <v>300</v>
       </c>
       <c r="F151" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B152" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C152" t="s">
         <v>301</v>
@@ -3697,10 +3967,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B153" t="s">
-        <v>312</v>
+        <v>434</v>
       </c>
       <c r="C153" t="s">
         <v>303</v>
@@ -3711,10 +3981,10 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="B154" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C154" t="s">
         <v>305</v>
@@ -3723,208 +3993,208 @@
         <v>306</v>
       </c>
       <c r="F154" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B155" t="s">
+        <v>368</v>
+      </c>
+      <c r="C155" t="s">
         <v>369</v>
       </c>
-      <c r="C155" t="s">
-        <v>370</v>
-      </c>
       <c r="E155" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B156" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C156" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E156" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B157" t="s">
         <v>62</v>
       </c>
       <c r="C157" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E157" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B158" t="s">
         <v>62</v>
       </c>
       <c r="C158" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E158" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B159" t="s">
+        <v>329</v>
+      </c>
+      <c r="C159" t="s">
+        <v>329</v>
+      </c>
+      <c r="E159" t="s">
         <v>330</v>
-      </c>
-      <c r="C159" t="s">
-        <v>330</v>
-      </c>
-      <c r="E159" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>365</v>
+      </c>
+      <c r="B160" t="s">
+        <v>367</v>
+      </c>
+      <c r="C160" t="s">
+        <v>331</v>
+      </c>
+      <c r="E160" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>365</v>
+      </c>
+      <c r="B161" t="s">
+        <v>367</v>
+      </c>
+      <c r="C161" t="s">
+        <v>333</v>
+      </c>
+      <c r="E161" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>365</v>
+      </c>
+      <c r="B162" t="s">
+        <v>367</v>
+      </c>
+      <c r="C162" t="s">
+        <v>335</v>
+      </c>
+      <c r="E162" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>365</v>
+      </c>
+      <c r="B163" t="s">
+        <v>367</v>
+      </c>
+      <c r="C163" t="s">
+        <v>337</v>
+      </c>
+      <c r="E163" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>365</v>
+      </c>
+      <c r="B164" t="s">
+        <v>367</v>
+      </c>
+      <c r="C164" t="s">
+        <v>339</v>
+      </c>
+      <c r="E164" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>365</v>
+      </c>
+      <c r="B165" t="s">
+        <v>367</v>
+      </c>
+      <c r="C165" t="s">
+        <v>341</v>
+      </c>
+      <c r="E165" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>365</v>
+      </c>
+      <c r="B166" t="s">
+        <v>367</v>
+      </c>
+      <c r="C166" t="s">
+        <v>343</v>
+      </c>
+      <c r="E166" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>365</v>
+      </c>
+      <c r="B167" t="s">
+        <v>367</v>
+      </c>
+      <c r="C167" t="s">
+        <v>345</v>
+      </c>
+      <c r="E167" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>365</v>
+      </c>
+      <c r="B168" t="s">
+        <v>367</v>
+      </c>
+      <c r="C168" t="s">
+        <v>347</v>
+      </c>
+      <c r="E168" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>366</v>
-      </c>
-      <c r="B160" t="s">
-        <v>368</v>
-      </c>
-      <c r="C160" t="s">
-        <v>332</v>
-      </c>
-      <c r="E160" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>366</v>
-      </c>
-      <c r="B161" t="s">
-        <v>368</v>
-      </c>
-      <c r="C161" t="s">
-        <v>334</v>
-      </c>
-      <c r="E161" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>366</v>
-      </c>
-      <c r="B162" t="s">
-        <v>368</v>
-      </c>
-      <c r="C162" t="s">
-        <v>336</v>
-      </c>
-      <c r="E162" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>366</v>
-      </c>
-      <c r="B163" t="s">
-        <v>368</v>
-      </c>
-      <c r="C163" t="s">
-        <v>338</v>
-      </c>
-      <c r="E163" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>366</v>
-      </c>
-      <c r="B164" t="s">
-        <v>368</v>
-      </c>
-      <c r="C164" t="s">
-        <v>340</v>
-      </c>
-      <c r="E164" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>366</v>
-      </c>
-      <c r="B165" t="s">
-        <v>368</v>
-      </c>
-      <c r="C165" t="s">
-        <v>342</v>
-      </c>
-      <c r="E165" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>366</v>
-      </c>
-      <c r="B166" t="s">
-        <v>368</v>
-      </c>
-      <c r="C166" t="s">
-        <v>344</v>
-      </c>
-      <c r="E166" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>366</v>
-      </c>
-      <c r="B167" t="s">
-        <v>368</v>
-      </c>
-      <c r="C167" t="s">
-        <v>346</v>
-      </c>
-      <c r="E167" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>366</v>
-      </c>
-      <c r="B168" t="s">
-        <v>368</v>
-      </c>
-      <c r="C168" t="s">
-        <v>348</v>
-      </c>
-      <c r="E168" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>367</v>
       </c>
       <c r="B169" t="s">
         <v>1</v>
@@ -3933,26 +4203,26 @@
         <v>2</v>
       </c>
       <c r="E169" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B170" t="s">
         <v>1</v>
       </c>
       <c r="C170" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E170" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B171" t="s">
         <v>1</v>
@@ -3961,12 +4231,12 @@
         <v>219</v>
       </c>
       <c r="E171" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B172" t="s">
         <v>1</v>
@@ -3975,161 +4245,749 @@
         <v>22</v>
       </c>
       <c r="E172" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B173" t="s">
         <v>1</v>
       </c>
       <c r="C173" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E173" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B174" t="s">
         <v>1</v>
       </c>
       <c r="C174" t="s">
+        <v>373</v>
+      </c>
+      <c r="E174" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>366</v>
+      </c>
+      <c r="B175" t="s">
+        <v>309</v>
+      </c>
+      <c r="C175" t="s">
+        <v>116</v>
+      </c>
+      <c r="E175" t="s">
+        <v>396</v>
+      </c>
+      <c r="F175" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>366</v>
+      </c>
+      <c r="B176" t="s">
+        <v>309</v>
+      </c>
+      <c r="C176" t="s">
+        <v>58</v>
+      </c>
+      <c r="E176" t="s">
+        <v>398</v>
+      </c>
+      <c r="F176" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>366</v>
+      </c>
+      <c r="B177" t="s">
+        <v>309</v>
+      </c>
+      <c r="C177" t="s">
+        <v>60</v>
+      </c>
+      <c r="E177" t="s">
+        <v>400</v>
+      </c>
+      <c r="F177" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>366</v>
+      </c>
+      <c r="B178" t="s">
+        <v>309</v>
+      </c>
+      <c r="C178" t="s">
+        <v>435</v>
+      </c>
+      <c r="E178" t="s">
+        <v>402</v>
+      </c>
+      <c r="F178" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>366</v>
+      </c>
+      <c r="B179" t="s">
+        <v>309</v>
+      </c>
+      <c r="C179" t="s">
+        <v>62</v>
+      </c>
+      <c r="E179" t="s">
+        <v>404</v>
+      </c>
+      <c r="F179" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>366</v>
+      </c>
+      <c r="B180" t="s">
+        <v>309</v>
+      </c>
+      <c r="C180" t="s">
+        <v>437</v>
+      </c>
+      <c r="E180" t="s">
+        <v>406</v>
+      </c>
+      <c r="F180" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>366</v>
+      </c>
+      <c r="B181" t="s">
+        <v>309</v>
+      </c>
+      <c r="C181" t="s">
+        <v>436</v>
+      </c>
+      <c r="E181" t="s">
+        <v>408</v>
+      </c>
+      <c r="F181" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>366</v>
+      </c>
+      <c r="B182" t="s">
+        <v>309</v>
+      </c>
+      <c r="C182" t="s">
+        <v>178</v>
+      </c>
+      <c r="E182" t="s">
+        <v>410</v>
+      </c>
+      <c r="F182" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>366</v>
+      </c>
+      <c r="B183" t="s">
+        <v>309</v>
+      </c>
+      <c r="C183" t="s">
+        <v>88</v>
+      </c>
+      <c r="E183" t="s">
+        <v>412</v>
+      </c>
+      <c r="F183" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" t="s">
+        <v>309</v>
+      </c>
+      <c r="C184" t="s">
+        <v>94</v>
+      </c>
+      <c r="E184" t="s">
+        <v>414</v>
+      </c>
+      <c r="F184" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>366</v>
+      </c>
+      <c r="B185" t="s">
+        <v>310</v>
+      </c>
+      <c r="C185" t="s">
+        <v>116</v>
+      </c>
+      <c r="E185" t="s">
         <v>374</v>
       </c>
-      <c r="E174" t="s">
+      <c r="F185" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>366</v>
+      </c>
+      <c r="B186" t="s">
+        <v>310</v>
+      </c>
+      <c r="C186" t="s">
+        <v>58</v>
+      </c>
+      <c r="E186" t="s">
+        <v>376</v>
+      </c>
+      <c r="F186" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>366</v>
+      </c>
+      <c r="B187" t="s">
+        <v>310</v>
+      </c>
+      <c r="C187" t="s">
+        <v>119</v>
+      </c>
+      <c r="E187" t="s">
+        <v>378</v>
+      </c>
+      <c r="F187" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>366</v>
+      </c>
+      <c r="B188" t="s">
+        <v>310</v>
+      </c>
+      <c r="C188" t="s">
+        <v>436</v>
+      </c>
+      <c r="E188" t="s">
+        <v>380</v>
+      </c>
+      <c r="F188" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>366</v>
+      </c>
+      <c r="B189" t="s">
+        <v>310</v>
+      </c>
+      <c r="C189" t="s">
+        <v>135</v>
+      </c>
+      <c r="E189" t="s">
+        <v>382</v>
+      </c>
+      <c r="F189" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>366</v>
+      </c>
+      <c r="B190" t="s">
+        <v>310</v>
+      </c>
+      <c r="C190" t="s">
+        <v>145</v>
+      </c>
+      <c r="E190" t="s">
+        <v>384</v>
+      </c>
+      <c r="F190" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>366</v>
+      </c>
+      <c r="B191" t="s">
+        <v>310</v>
+      </c>
+      <c r="C191" t="s">
+        <v>94</v>
+      </c>
+      <c r="E191" t="s">
+        <v>386</v>
+      </c>
+      <c r="F191" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>366</v>
+      </c>
+      <c r="B192" t="s">
+        <v>310</v>
+      </c>
+      <c r="C192" t="s">
+        <v>166</v>
+      </c>
+      <c r="E192" t="s">
+        <v>388</v>
+      </c>
+      <c r="F192" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>366</v>
+      </c>
+      <c r="B193" t="s">
+        <v>310</v>
+      </c>
+      <c r="C193" t="s">
+        <v>170</v>
+      </c>
+      <c r="E193" t="s">
+        <v>390</v>
+      </c>
+      <c r="F193" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>366</v>
+      </c>
+      <c r="B194" t="s">
+        <v>310</v>
+      </c>
+      <c r="C194" t="s">
+        <v>178</v>
+      </c>
+      <c r="E194" t="s">
+        <v>392</v>
+      </c>
+      <c r="F194" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>366</v>
+      </c>
+      <c r="B195" t="s">
+        <v>310</v>
+      </c>
+      <c r="C195" t="s">
+        <v>181</v>
+      </c>
+      <c r="E195" t="s">
+        <v>394</v>
+      </c>
+      <c r="F195" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>366</v>
+      </c>
+      <c r="B196" t="s">
+        <v>311</v>
+      </c>
+      <c r="C196" t="s">
+        <v>194</v>
+      </c>
+      <c r="E196" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>367</v>
-      </c>
-      <c r="B175" t="s">
-        <v>311</v>
-      </c>
-      <c r="C175" t="s">
-        <v>194</v>
-      </c>
-      <c r="E175" t="s">
+      <c r="F196" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>366</v>
+      </c>
+      <c r="B197" t="s">
+        <v>311</v>
+      </c>
+      <c r="C197" t="s">
+        <v>116</v>
+      </c>
+      <c r="E197" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>367</v>
-      </c>
-      <c r="B176" t="s">
-        <v>311</v>
-      </c>
-      <c r="C176" t="s">
-        <v>116</v>
-      </c>
-      <c r="E176" t="s">
+      <c r="F197" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>366</v>
+      </c>
+      <c r="B198" t="s">
+        <v>311</v>
+      </c>
+      <c r="C198" t="s">
+        <v>209</v>
+      </c>
+      <c r="E198" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>367</v>
-      </c>
-      <c r="B177" t="s">
-        <v>311</v>
-      </c>
-      <c r="C177" t="s">
+      <c r="F198" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>366</v>
+      </c>
+      <c r="B199" t="s">
+        <v>311</v>
+      </c>
+      <c r="C199" t="s">
+        <v>217</v>
+      </c>
+      <c r="E199" t="s">
+        <v>358</v>
+      </c>
+      <c r="F199" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>366</v>
+      </c>
+      <c r="B200" t="s">
+        <v>311</v>
+      </c>
+      <c r="C200" t="s">
+        <v>221</v>
+      </c>
+      <c r="E200" t="s">
+        <v>359</v>
+      </c>
+      <c r="F200" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>366</v>
+      </c>
+      <c r="B201" t="s">
+        <v>311</v>
+      </c>
+      <c r="C201" t="s">
+        <v>230</v>
+      </c>
+      <c r="E201" t="s">
+        <v>360</v>
+      </c>
+      <c r="F201" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>366</v>
+      </c>
+      <c r="B202" t="s">
+        <v>311</v>
+      </c>
+      <c r="C202" t="s">
+        <v>238</v>
+      </c>
+      <c r="E202" t="s">
+        <v>361</v>
+      </c>
+      <c r="F202" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>366</v>
+      </c>
+      <c r="B203" t="s">
+        <v>311</v>
+      </c>
+      <c r="C203" t="s">
+        <v>234</v>
+      </c>
+      <c r="E203" t="s">
+        <v>362</v>
+      </c>
+      <c r="F203" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>366</v>
+      </c>
+      <c r="B204" t="s">
+        <v>311</v>
+      </c>
+      <c r="C204" t="s">
+        <v>266</v>
+      </c>
+      <c r="E204" t="s">
+        <v>363</v>
+      </c>
+      <c r="F204" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>432</v>
+      </c>
+      <c r="B205" t="s">
+        <v>434</v>
+      </c>
+      <c r="C205" t="s">
+        <v>282</v>
+      </c>
+      <c r="E205" t="s">
+        <v>418</v>
+      </c>
+      <c r="F205" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>432</v>
+      </c>
+      <c r="B206" t="s">
+        <v>434</v>
+      </c>
+      <c r="C206" t="s">
         <v>209</v>
       </c>
-      <c r="E177" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>367</v>
-      </c>
-      <c r="B178" t="s">
-        <v>311</v>
-      </c>
-      <c r="C178" t="s">
-        <v>217</v>
-      </c>
-      <c r="E178" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>367</v>
-      </c>
-      <c r="B179" t="s">
-        <v>311</v>
-      </c>
-      <c r="C179" t="s">
-        <v>221</v>
-      </c>
-      <c r="E179" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>367</v>
-      </c>
-      <c r="B180" t="s">
-        <v>311</v>
-      </c>
-      <c r="C180" t="s">
-        <v>230</v>
-      </c>
-      <c r="E180" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>367</v>
-      </c>
-      <c r="B181" t="s">
-        <v>311</v>
-      </c>
-      <c r="C181" t="s">
-        <v>238</v>
-      </c>
-      <c r="E181" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>367</v>
-      </c>
-      <c r="B182" t="s">
-        <v>311</v>
-      </c>
-      <c r="C182" t="s">
-        <v>234</v>
-      </c>
-      <c r="E182" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>367</v>
-      </c>
-      <c r="B183" t="s">
-        <v>311</v>
-      </c>
-      <c r="C183" t="s">
-        <v>266</v>
-      </c>
-      <c r="E183" t="s">
-        <v>364</v>
+      <c r="E206" t="s">
+        <v>420</v>
+      </c>
+      <c r="F206" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>432</v>
+      </c>
+      <c r="B207" t="s">
+        <v>434</v>
+      </c>
+      <c r="C207" t="s">
+        <v>285</v>
+      </c>
+      <c r="E207" t="s">
+        <v>422</v>
+      </c>
+      <c r="F207" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>432</v>
+      </c>
+      <c r="B208" t="s">
+        <v>434</v>
+      </c>
+      <c r="C208" t="s">
+        <v>287</v>
+      </c>
+      <c r="E208" t="s">
+        <v>424</v>
+      </c>
+      <c r="F208" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>432</v>
+      </c>
+      <c r="B209" t="s">
+        <v>434</v>
+      </c>
+      <c r="C209" t="s">
+        <v>294</v>
+      </c>
+      <c r="E209" t="s">
+        <v>426</v>
+      </c>
+      <c r="F209" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>432</v>
+      </c>
+      <c r="B210" t="s">
+        <v>434</v>
+      </c>
+      <c r="C210" t="s">
+        <v>439</v>
+      </c>
+      <c r="E210" t="s">
+        <v>428</v>
+      </c>
+      <c r="F210" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>432</v>
+      </c>
+      <c r="B211" t="s">
+        <v>312</v>
+      </c>
+      <c r="C211" t="s">
+        <v>312</v>
+      </c>
+      <c r="E211" t="s">
+        <v>430</v>
+      </c>
+      <c r="F211" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>433</v>
+      </c>
+      <c r="B212" t="s">
+        <v>438</v>
+      </c>
+      <c r="C212" t="s">
+        <v>438</v>
+      </c>
+      <c r="E212" t="s">
+        <v>416</v>
+      </c>
+      <c r="F212" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>433</v>
+      </c>
+      <c r="B213" t="s">
+        <v>451</v>
+      </c>
+      <c r="C213" t="s">
+        <v>452</v>
+      </c>
+      <c r="E213" t="s">
+        <v>453</v>
+      </c>
+      <c r="F213" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>433</v>
+      </c>
+      <c r="B214" t="s">
+        <v>451</v>
+      </c>
+      <c r="C214" t="s">
+        <v>457</v>
+      </c>
+      <c r="E214" t="s">
+        <v>455</v>
+      </c>
+      <c r="F214" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>433</v>
+      </c>
+      <c r="B215" t="s">
+        <v>451</v>
+      </c>
+      <c r="C215" t="s">
+        <v>458</v>
+      </c>
+      <c r="E215" t="s">
+        <v>459</v>
+      </c>
+      <c r="F215" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>433</v>
+      </c>
+      <c r="B216" t="s">
+        <v>451</v>
+      </c>
+      <c r="C216" t="s">
+        <v>461</v>
+      </c>
+      <c r="E216" t="s">
+        <v>462</v>
+      </c>
+      <c r="F216" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>